<commit_message>
added sql pandas codes
</commit_message>
<xml_diff>
--- a/codes/other/weather_data.xlsx
+++ b/codes/other/weather_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JD_Sharif\Python\Python_DataScience\github\codes\02_csv_processing\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\JD_Sharif\Python\Python_DataScience\github\codes\other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D26E36BA-E560-4D25-8BF7-473BBDCB6B7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE4A374B-6AA8-4B93-8CED-11F8EDEDAE37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3060" yWindow="-10908" windowWidth="17496" windowHeight="10296"/>
+    <workbookView xWindow="-120" yWindow="-11640" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weather_data" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -898,10 +898,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>

</xml_diff>